<commit_message>
ajout du début des messages de 2022
</commit_message>
<xml_diff>
--- a/photos_used.xlsx
+++ b/photos_used.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9efc16f3edaae178/Documents/Jean/Code/PourMaAbi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{9DB7CAEB-5026-49BE-AD4E-ED97495BBACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5D25D96-648C-4A4A-BCCB-8BBD754710CA}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="8_{9DB7CAEB-5026-49BE-AD4E-ED97495BBACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2F0AF8F-1038-4B76-B457-ADD458971FC7}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-15" windowWidth="17985" windowHeight="15135" xr2:uid="{C5E1D242-CC0D-41A9-A10A-C7BA64C13ED2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="24300" xr2:uid="{C5E1D242-CC0D-41A9-A10A-C7BA64C13ED2}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -391,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA826A81-1E99-46D9-838D-2B332863AD19}">
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +461,7 @@
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>14</v>
       </c>
     </row>
@@ -560,7 +556,7 @@
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>33</v>
       </c>
     </row>
@@ -595,8 +591,123 @@
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="1">
         <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout des mots 2022
</commit_message>
<xml_diff>
--- a/photos_used.xlsx
+++ b/photos_used.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9efc16f3edaae178/Documents/Jean/Code/PourMaAbi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{9DB7CAEB-5026-49BE-AD4E-ED97495BBACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D864A22-0037-4094-8BE2-20B8FF58C0A0}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{9DB7CAEB-5026-49BE-AD4E-ED97495BBACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA118789-83BA-414F-A761-A18DCB44F0EA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17100" windowHeight="24300" xr2:uid="{C5E1D242-CC0D-41A9-A10A-C7BA64C13ED2}"/>
+    <workbookView xWindow="28680" yWindow="405" windowWidth="29040" windowHeight="15195" xr2:uid="{C5E1D242-CC0D-41A9-A10A-C7BA64C13ED2}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -387,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA826A81-1E99-46D9-838D-2B332863AD19}">
-  <dimension ref="A1:A63"/>
+  <dimension ref="A1:A64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:A48"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,32 +561,32 @@
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="1">
         <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="1">
         <v>39</v>
       </c>
     </row>
@@ -636,62 +636,62 @@
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="1">
         <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="1">
         <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="1">
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="1">
         <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="1">
         <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="1">
         <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="1">
         <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="1">
         <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" s="1">
         <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="1">
         <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="1">
         <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" s="1">
         <v>60</v>
       </c>
     </row>
@@ -701,13 +701,18 @@
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" s="1">
         <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout de la photo 65
</commit_message>
<xml_diff>
--- a/photos_used.xlsx
+++ b/photos_used.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9efc16f3edaae178/Documents/Jean/Code/PourMaAbi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{9DB7CAEB-5026-49BE-AD4E-ED97495BBACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA118789-83BA-414F-A761-A18DCB44F0EA}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{9DB7CAEB-5026-49BE-AD4E-ED97495BBACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6C70DF2-1AB6-4706-84C5-C762C24660AD}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="405" windowWidth="29040" windowHeight="15195" xr2:uid="{C5E1D242-CC0D-41A9-A10A-C7BA64C13ED2}"/>
+    <workbookView xWindow="16080" yWindow="10695" windowWidth="29040" windowHeight="15195" xr2:uid="{C5E1D242-CC0D-41A9-A10A-C7BA64C13ED2}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -387,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA826A81-1E99-46D9-838D-2B332863AD19}">
-  <dimension ref="A1:A64"/>
+  <dimension ref="A1:A65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,6 +715,11 @@
         <v>64</v>
       </c>
     </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>